<commit_message>
fixed shader distortion mesh method
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,24 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>ms</t>
   </si>
   <si>
     <t>power2</t>
-  </si>
-  <si>
-    <t>cull compare</t>
-  </si>
-  <si>
-    <t>frust</t>
-  </si>
-  <si>
-    <t>dist</t>
-  </si>
-  <si>
-    <t>orientation</t>
   </si>
   <si>
     <t>tess falloff</t>
@@ -62,6 +50,24 @@
   </si>
   <si>
     <t>push</t>
+  </si>
+  <si>
+    <t>ppStage compare</t>
+  </si>
+  <si>
+    <t>passthrough</t>
+  </si>
+  <si>
+    <t>everything in frag</t>
+  </si>
+  <si>
+    <t>shader Mesh</t>
+  </si>
+  <si>
+    <t>precalc mesh</t>
+  </si>
+  <si>
+    <t>stencil mesh</t>
   </si>
 </sst>
 </file>
@@ -140,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -155,6 +161,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -213,7 +221,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Culling vs No Culling</a:t>
+              <a:t>UBO per Mesh vs Push Constant</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -862,7 +870,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Culling Comparison</a:t>
+              <a:t>TECHNIQUE VS TIME</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -920,208 +928,10 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="2"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Frustum</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$4:$B$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>700</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>900</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1100</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1300</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$14:$C$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1.4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30.3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>200</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9CA7-4C1E-832E-48A6230DB0B8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Distance</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$4:$B$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>700</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>900</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1100</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1300</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$14:$D$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1.7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41.4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>333</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9CA7-4C1E-832E-48A6230DB0B8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Orientation</c:v>
+            <c:v>Passthrough</c:v>
           </c:tx>
           <c:spPr>
             <a:gradFill rotWithShape="1">
@@ -1164,21 +974,12 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$14:$E$17</c:f>
+              <c:f>Sheet1!$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32.299999999999997</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>250</c:v>
+                  <c:v>5.26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1186,6 +987,258 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-9CA7-4C1E-832E-48A6230DB0B8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>All in frag</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5.29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8B9E-4921-A4F1-A677DE1AF386}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Shader Mesh</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5.26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8B9E-4921-A4F1-A677DE1AF386}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Precalc Mesh</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5.31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8B9E-4921-A4F1-A677DE1AF386}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Stencil Mesh</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8B9E-4921-A4F1-A677DE1AF386}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1242,13 +1295,9 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1800"/>
-                  <a:t>Num Grass</a:t>
+                  <a:t>Technique</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1800" baseline="0"/>
-                  <a:t> Blades (power of 2)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" sz="1800"/>
+                <a:endParaRPr lang="en-US" sz="1800" baseline="0"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1449,644 +1498,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.31901323636112527"/>
           <c:y val="0.87129652988151685"/>
-          <c:w val="0.45552151979458272"/>
-          <c:h val="6.8684133676935447E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="95000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Tessalation Falloff vs No Falloff</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.11410685703083236"/>
-          <c:y val="0.12997359154929577"/>
-          <c:w val="0.86389534274918967"/>
-          <c:h val="0.5970335546745037"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Falloff</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$4:$B$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>700</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>900</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1100</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1300</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$21:$C$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15.6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>111</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7839-42D5-8AB0-01E480395182}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>No Falloff</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$4:$B$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>700</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>900</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1100</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1300</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$21:$D$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1.4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>18.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>142</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7839-42D5-8AB0-01E480395182}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="494948056"/>
-        <c:axId val="494949368"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="494948056"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1800"/>
-                  <a:t>Num Grass</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1800" baseline="0"/>
-                  <a:t> Blades (power of 2)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" sz="1800"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="494949368"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="494949368"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1600"/>
-                  <a:t>TIME (ms)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="494948056"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="25400">
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.29160778959522188"/>
-          <c:y val="0.88206579000366736"/>
-          <c:w val="0.46024014228999355"/>
-          <c:h val="6.8208847328778299E-2"/>
+          <c:w val="0.68098681068695832"/>
+          <c:h val="6.8486094396081429E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2245,46 +1658,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
   <cs:axisTitle>
@@ -3289,508 +2662,6 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3801,8 +2672,8 @@
       <xdr:rowOff>84388</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>303900</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>142240</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>27542</xdr:rowOff>
     </xdr:to>
@@ -3864,44 +2735,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>550843</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>165253</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>157008</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>108407</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87F9CF71-81AD-4C30-A3E5-C196A0F9D9AF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4175,8 +3008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="C12" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4187,7 +3020,7 @@
     <col min="4" max="4" width="20.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" style="1" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -4197,16 +3030,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="7"/>
@@ -4215,7 +3048,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
       <c r="B3" s="10" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>0</v>
@@ -4322,19 +3155,23 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8"/>
+        <v>13</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
@@ -4349,70 +3186,54 @@
       <c r="E13" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8"/>
+      <c r="F13" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="10">
-        <v>13</v>
-      </c>
-      <c r="C14" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="D14" s="5">
-        <v>1.7</v>
+        <v>1</v>
+      </c>
+      <c r="C14" s="11">
+        <v>5.26</v>
+      </c>
+      <c r="D14" s="12">
+        <v>5.29</v>
       </c>
       <c r="E14" s="6">
-        <v>1.4</v>
-      </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
+        <v>5.26</v>
+      </c>
+      <c r="F14" s="7">
+        <v>5.31</v>
+      </c>
+      <c r="G14" s="8">
+        <v>4.7</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="10">
-        <v>16</v>
-      </c>
-      <c r="C15" s="4">
-        <v>4.5</v>
-      </c>
-      <c r="D15" s="5">
-        <v>5.8</v>
-      </c>
-      <c r="E15" s="6">
-        <v>4.5</v>
-      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
       <c r="F15" s="7"/>
       <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="10">
-        <v>19</v>
-      </c>
-      <c r="C16" s="4">
-        <v>30.3</v>
-      </c>
-      <c r="D16" s="5">
-        <v>41.4</v>
-      </c>
-      <c r="E16" s="6">
-        <v>32.299999999999997</v>
-      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
       <c r="F16" s="7"/>
       <c r="G16" s="8"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="3">
-        <v>22</v>
-      </c>
-      <c r="C17" s="4">
-        <v>200</v>
-      </c>
-      <c r="D17" s="5">
-        <v>333</v>
-      </c>
-      <c r="E17" s="6">
-        <v>250</v>
-      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
     </row>
@@ -4421,13 +3242,13 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="10" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="7"/>

</xml_diff>

<commit_message>
added support for adaptive quality filtering, updated readme
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>ms</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>stencil mesh</t>
+  </si>
+  <si>
+    <t>stencil mesh + hole fill</t>
   </si>
 </sst>
 </file>
@@ -1183,7 +1186,7 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>Stencil Mesh</c:v>
+            <c:v>Stencil</c:v>
           </c:tx>
           <c:spPr>
             <a:gradFill rotWithShape="1">
@@ -1239,6 +1242,69 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-8B9E-4921-A4F1-A677DE1AF386}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Stencil + Fill</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B176-4F56-9C63-C1C321073C81}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1496,10 +1562,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.31901323636112527"/>
-          <c:y val="0.87129652988151685"/>
-          <c:w val="0.68098681068695832"/>
-          <c:h val="6.8486094396081429E-2"/>
+          <c:x val="3.0585680697121469E-2"/>
+          <c:y val="0.81993467905936823"/>
+          <c:w val="0.93095731815408922"/>
+          <c:h val="0.11984800450571449"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2667,15 +2733,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>302965</xdr:colOff>
+      <xdr:colOff>272485</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>84388</xdr:rowOff>
+      <xdr:rowOff>64068</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>142240</xdr:colOff>
+      <xdr:colOff>111760</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>27542</xdr:rowOff>
+      <xdr:rowOff>7222</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3006,10 +3072,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C12" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="C14" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="Z27" sqref="Z27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3024,11 +3090,11 @@
     <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="9"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
@@ -3045,7 +3111,7 @@
       <c r="F2" s="7"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
       <c r="B3" s="10" t="s">
         <v>5</v>
@@ -3060,7 +3126,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" s="3">
         <v>500</v>
       </c>
@@ -3074,7 +3140,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
       <c r="B5" s="3">
         <v>700</v>
@@ -3089,7 +3155,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>900</v>
       </c>
@@ -3103,7 +3169,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" s="10">
         <v>1100</v>
       </c>
@@ -3117,7 +3183,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" s="10">
         <v>1300</v>
       </c>
@@ -3131,7 +3197,7 @@
       <c r="F8" s="7"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <v>1500</v>
       </c>
@@ -3142,7 +3208,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1700</v>
       </c>
@@ -3153,7 +3219,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
         <v>10</v>
       </c>
@@ -3172,8 +3238,11 @@
       <c r="G12" s="15" t="s">
         <v>15</v>
       </c>
+      <c r="H12" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
         <v>1</v>
       </c>
@@ -3192,8 +3261,11 @@
       <c r="G13" s="15" t="s">
         <v>0</v>
       </c>
+      <c r="H13" s="9" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" s="10">
         <v>1</v>
       </c>
@@ -3212,8 +3284,11 @@
       <c r="G14" s="8">
         <v>4.7</v>
       </c>
+      <c r="H14" s="1">
+        <v>5.2</v>
+      </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" s="10"/>
       <c r="C15" s="4"/>
       <c r="D15" s="5"/>
@@ -3221,7 +3296,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B16" s="10"/>
       <c r="C16" s="4"/>
       <c r="D16" s="5"/>

</xml_diff>

<commit_message>
update readme, almost there to adaptive quality
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>ms</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>stencil mesh + hole fill</t>
+  </si>
+  <si>
+    <t>Optimized stencil + hole fill</t>
   </si>
 </sst>
 </file>
@@ -982,7 +985,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5.26</c:v>
+                  <c:v>4.5999999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1045,7 +1048,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5.29</c:v>
+                  <c:v>4.5999999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1108,7 +1111,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5.26</c:v>
+                  <c:v>4.5999999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1171,7 +1174,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5.31</c:v>
+                  <c:v>4.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1234,7 +1237,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4.7</c:v>
+                  <c:v>3.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1297,7 +1300,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5.2</c:v>
+                  <c:v>5.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1305,6 +1308,72 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B176-4F56-9C63-C1C321073C81}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>Opt Stencil+Fill</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-81DF-4E83-8019-E9AF4AFCF484}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1564,8 +1633,8 @@
           <c:yMode val="edge"/>
           <c:x val="3.0585680697121469E-2"/>
           <c:y val="0.81993467905936823"/>
-          <c:w val="0.93095731815408922"/>
-          <c:h val="0.11984800450571449"/>
+          <c:w val="0.73749122321147498"/>
+          <c:h val="0.13291730115192865"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2732,16 +2801,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>272485</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>242005</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>64068</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>111760</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>7222</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>81280</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>126034</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2770,16 +2839,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>330506</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>249226</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>64265</xdr:rowOff>
+      <xdr:rowOff>54105</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>331441</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>7419</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>250161</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>180139</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3072,10 +3141,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C14" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="Z27" sqref="Z27"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3090,11 +3159,11 @@
     <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="9"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
@@ -3111,7 +3180,7 @@
       <c r="F2" s="7"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
       <c r="B3" s="10" t="s">
         <v>5</v>
@@ -3126,7 +3195,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="3">
         <v>500</v>
       </c>
@@ -3140,7 +3209,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
       <c r="B5" s="3">
         <v>700</v>
@@ -3155,7 +3224,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>900</v>
       </c>
@@ -3169,7 +3238,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" s="10">
         <v>1100</v>
       </c>
@@ -3183,7 +3252,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" s="10">
         <v>1300</v>
       </c>
@@ -3197,7 +3266,7 @@
       <c r="F8" s="7"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <v>1500</v>
       </c>
@@ -3208,7 +3277,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1700</v>
       </c>
@@ -3219,7 +3288,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
         <v>10</v>
       </c>
@@ -3241,8 +3310,11 @@
       <c r="H12" s="9" t="s">
         <v>16</v>
       </c>
+      <c r="I12" s="9" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
         <v>1</v>
       </c>
@@ -3264,31 +3336,37 @@
       <c r="H13" s="9" t="s">
         <v>0</v>
       </c>
+      <c r="I13" s="9" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="10">
         <v>1</v>
       </c>
       <c r="C14" s="11">
-        <v>5.26</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D14" s="12">
-        <v>5.29</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E14" s="6">
-        <v>5.26</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="F14" s="7">
-        <v>5.31</v>
+        <v>4.7</v>
       </c>
       <c r="G14" s="8">
-        <v>4.7</v>
+        <v>3.8</v>
       </c>
       <c r="H14" s="1">
-        <v>5.2</v>
+        <v>5.3</v>
+      </c>
+      <c r="I14" s="1">
+        <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="10"/>
       <c r="C15" s="4"/>
       <c r="D15" s="5"/>
@@ -3296,7 +3374,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" s="10"/>
       <c r="C16" s="4"/>
       <c r="D16" s="5"/>

</xml_diff>